<commit_message>
still setting up the repo
</commit_message>
<xml_diff>
--- a/project/excel/definedtermset_profile.xlsx
+++ b/project/excel/definedtermset_profile.xlsx
@@ -451,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,46 +462,21 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>primary_email</t>
+          <t>id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>name</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
-        <is>
-          <t>age_in_years</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>vital_status</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ALIVE,DEAD,UNKNOWN"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update DefinedTern and DefinedTermSet classes and regen project
</commit_message>
<xml_diff>
--- a/project/excel/definedtermset_profile.xlsx
+++ b/project/excel/definedtermset_profile.xlsx
@@ -7,9 +7,11 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Person" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="PersonCollection" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Thing" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Intangible" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="CreativeWork" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="DefinedTerm" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="DefinedTermSet" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -415,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -431,12 +433,27 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>alternateName</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sameAs</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>url</t>
         </is>
       </c>
     </row>
@@ -451,7 +468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,12 +484,27 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>alternateName</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sameAs</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>url</t>
         </is>
       </c>
     </row>
@@ -487,7 +519,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,7 +530,149 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>entries</t>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>alternateName</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>sameAs</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>inDefinedTermSet</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>termCode</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>alternateName</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>sameAs</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>hasDefinedTerm</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>alternateName</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>sameAs</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>url</t>
         </is>
       </c>
     </row>

</xml_diff>